<commit_message>
finalizei ajustes de modelagem e dash
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/vendas_atipicas.xlsx
+++ b/dados/ADD/Dados_ADD_PF/vendas_atipicas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="75">
   <si>
     <t>data</t>
   </si>
@@ -25,6 +25,9 @@
     <t>cliente</t>
   </si>
   <si>
+    <t>id_venda</t>
+  </si>
+  <si>
     <t>id_produto</t>
   </si>
   <si>
@@ -34,6 +37,12 @@
     <t>estoque_atualizado</t>
   </si>
   <si>
+    <t>media_vendas</t>
+  </si>
+  <si>
+    <t>desvio_padrao</t>
+  </si>
+  <si>
     <t>2025-05-28</t>
   </si>
   <si>
@@ -107,6 +116,60 @@
   </si>
   <si>
     <t>MAP SERVICOS DE CONSERVACAO - EIRELI</t>
+  </si>
+  <si>
+    <t>52290256</t>
+  </si>
+  <si>
+    <t>52293818</t>
+  </si>
+  <si>
+    <t>52321934</t>
+  </si>
+  <si>
+    <t>52169486</t>
+  </si>
+  <si>
+    <t>52287381</t>
+  </si>
+  <si>
+    <t>52399913</t>
+  </si>
+  <si>
+    <t>52460562</t>
+  </si>
+  <si>
+    <t>52454962</t>
+  </si>
+  <si>
+    <t>52483994</t>
+  </si>
+  <si>
+    <t>52179187</t>
+  </si>
+  <si>
+    <t>52511013</t>
+  </si>
+  <si>
+    <t>52178397</t>
+  </si>
+  <si>
+    <t>52589494</t>
+  </si>
+  <si>
+    <t>52546760</t>
+  </si>
+  <si>
+    <t>52630305</t>
+  </si>
+  <si>
+    <t>52349545</t>
+  </si>
+  <si>
+    <t>52688164</t>
+  </si>
+  <si>
+    <t>52676511</t>
   </si>
   <si>
     <t>SABONETE LIQUIDO BRILLANO ERVA DOCE  5L</t>
@@ -533,13 +596,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -558,485 +621,710 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2">
         <v>13881226</v>
       </c>
-      <c r="E2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2">
+      <c r="F2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="H2">
+        <v>3.25</v>
+      </c>
+      <c r="I2">
+        <v>4.31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3">
         <v>14589858</v>
       </c>
-      <c r="E3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3">
+      <c r="F3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3">
         <v>58</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="H3">
+        <v>14.4</v>
+      </c>
+      <c r="I3">
+        <v>16.86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>148</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4">
         <v>31186309</v>
       </c>
-      <c r="E4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4">
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4">
         <v>122</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="H4">
+        <v>8.82</v>
+      </c>
+      <c r="I4">
+        <v>14.65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5">
         <v>11905183</v>
       </c>
-      <c r="E5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5">
+      <c r="F5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="H5">
+        <v>2.65</v>
+      </c>
+      <c r="I5">
+        <v>2.81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6">
         <v>16175304</v>
       </c>
-      <c r="E6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6">
+      <c r="F6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6">
         <v>279</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="H6">
+        <v>6.14</v>
+      </c>
+      <c r="I6">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>160</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7">
         <v>11939672</v>
       </c>
-      <c r="E7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7">
+      <c r="F7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7">
         <v>131</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="H7">
+        <v>9.550000000000001</v>
+      </c>
+      <c r="I7">
+        <v>27.02</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8">
         <v>27104217</v>
       </c>
-      <c r="E8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8">
+      <c r="F8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="H8">
+        <v>2.15</v>
+      </c>
+      <c r="I8">
+        <v>2.87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>120</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9">
         <v>17093168</v>
       </c>
-      <c r="E9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9">
+      <c r="F9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="H9">
+        <v>18.55</v>
+      </c>
+      <c r="I9">
+        <v>21.46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10">
         <v>13451851</v>
       </c>
-      <c r="E10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10">
+      <c r="F10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10">
         <v>441</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="H10">
+        <v>6.88</v>
+      </c>
+      <c r="I10">
+        <v>12.13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>50</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11">
         <v>14979850</v>
       </c>
-      <c r="E11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11">
+      <c r="F11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11">
         <v>148</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="H11">
+        <v>5.51</v>
+      </c>
+      <c r="I11">
+        <v>8.82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>72</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12">
         <v>26329148</v>
       </c>
-      <c r="E12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12">
+      <c r="F12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12">
         <v>617</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="H12">
+        <v>11.95</v>
+      </c>
+      <c r="I12">
+        <v>13.73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13">
         <v>12919709</v>
       </c>
-      <c r="E13" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13">
+      <c r="F13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="H13">
+        <v>2.5</v>
+      </c>
+      <c r="I13">
+        <v>3.18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14">
         <v>16921300</v>
       </c>
-      <c r="E14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14">
+      <c r="F14" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="H14">
+        <v>3.29</v>
+      </c>
+      <c r="I14">
+        <v>3.86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15">
         <v>17737776</v>
       </c>
-      <c r="E15" t="s">
-        <v>44</v>
-      </c>
-      <c r="F15">
+      <c r="F15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="H15">
+        <v>4.49</v>
+      </c>
+      <c r="I15">
+        <v>7.01</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B16">
         <v>500</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16">
+        <v>27</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16">
         <v>14667825</v>
       </c>
-      <c r="E16" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16">
+      <c r="F16" t="s">
+        <v>66</v>
+      </c>
+      <c r="G16">
         <v>1936</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="H16">
+        <v>38.69</v>
+      </c>
+      <c r="I16">
+        <v>82.45999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B17">
         <v>89</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17">
         <v>19006434</v>
       </c>
-      <c r="E17" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17">
+      <c r="F17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G17">
         <v>555</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="H17">
+        <v>10.71</v>
+      </c>
+      <c r="I17">
+        <v>15.81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B18">
         <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18">
+        <v>26</v>
+      </c>
+      <c r="D18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18">
         <v>14413867</v>
       </c>
-      <c r="E18" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18">
+      <c r="F18" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18">
         <v>-1</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="H18">
+        <v>3.91</v>
+      </c>
+      <c r="I18">
+        <v>6.15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B19">
         <v>500</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19">
+        <v>28</v>
+      </c>
+      <c r="D19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19">
         <v>32130390</v>
       </c>
-      <c r="E19" t="s">
-        <v>48</v>
-      </c>
-      <c r="F19">
+      <c r="F19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19">
         <v>5653</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="H19">
+        <v>21.78</v>
+      </c>
+      <c r="I19">
+        <v>52.03</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B20">
         <v>120</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20">
+        <v>29</v>
+      </c>
+      <c r="D20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20">
         <v>28503269</v>
       </c>
-      <c r="E20" t="s">
-        <v>49</v>
-      </c>
-      <c r="F20">
+      <c r="F20" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20">
         <v>-28</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="H20">
+        <v>16.22</v>
+      </c>
+      <c r="I20">
+        <v>21.49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B21">
         <v>200</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21">
+        <v>30</v>
+      </c>
+      <c r="D21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21">
         <v>19792364</v>
       </c>
-      <c r="E21" t="s">
-        <v>50</v>
-      </c>
-      <c r="F21">
+      <c r="F21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21">
         <v>-5</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="H21">
+        <v>21.77</v>
+      </c>
+      <c r="I21">
+        <v>32.94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B22">
         <v>320</v>
       </c>
       <c r="C22" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22">
+        <v>31</v>
+      </c>
+      <c r="D22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22">
         <v>28631402</v>
       </c>
-      <c r="E22" t="s">
-        <v>51</v>
-      </c>
-      <c r="F22">
+      <c r="F22" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="H22">
+        <v>38.68</v>
+      </c>
+      <c r="I22">
+        <v>62.08</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B23">
         <v>100</v>
       </c>
       <c r="C23" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23">
+        <v>31</v>
+      </c>
+      <c r="D23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23">
         <v>14589858</v>
       </c>
-      <c r="E23" t="s">
-        <v>32</v>
-      </c>
-      <c r="F23">
+      <c r="F23" t="s">
+        <v>53</v>
+      </c>
+      <c r="G23">
         <v>58</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="H23">
+        <v>14.4</v>
+      </c>
+      <c r="I23">
+        <v>16.86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B24">
         <v>70</v>
       </c>
       <c r="C24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24">
+        <v>32</v>
+      </c>
+      <c r="D24" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24">
         <v>30240035</v>
       </c>
-      <c r="E24" t="s">
-        <v>52</v>
-      </c>
-      <c r="F24">
+      <c r="F24" t="s">
+        <v>73</v>
+      </c>
+      <c r="G24">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="H24">
+        <v>12.78</v>
+      </c>
+      <c r="I24">
+        <v>13.39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B25">
         <v>30</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25">
+        <v>33</v>
+      </c>
+      <c r="D25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25">
         <v>11939645</v>
       </c>
-      <c r="E25" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25">
+      <c r="F25" t="s">
+        <v>74</v>
+      </c>
+      <c r="G25">
         <v>162</v>
+      </c>
+      <c r="H25">
+        <v>4.36</v>
+      </c>
+      <c r="I25">
+        <v>4.81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>